<commit_message>
Fixed orientation of ws2812b-mini LEDs in PnP files. fixed naming of x2 BoM and PnP files.
</commit_message>
<xml_diff>
--- a/cam/LED-plus35-SHIM_2021-09-07-PnP.xlsx
+++ b/cam/LED-plus35-SHIM_2021-09-07-PnP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AG\Documents\EAGLE\projects\LED-SHIM\cam\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98FF195A-5FAA-4E4F-8254-800611D8E0D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFE253DA-3F59-4F21-BD13-72E06712E6E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1140" yWindow="1050" windowWidth="17320" windowHeight="19950" xr2:uid="{226530C8-5020-45DB-AF73-7671C41FB870}"/>
   </bookViews>
@@ -850,7 +850,7 @@
   <dimension ref="A1:E132"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1061,7 +1061,7 @@
         <v>71</v>
       </c>
       <c r="E12" s="1">
-        <v>90</v>
+        <v>270</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
@@ -1078,7 +1078,7 @@
         <v>71</v>
       </c>
       <c r="E13" s="1">
-        <v>90</v>
+        <v>270</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
@@ -1095,7 +1095,7 @@
         <v>71</v>
       </c>
       <c r="E14" s="1">
-        <v>90</v>
+        <v>270</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
@@ -1112,7 +1112,7 @@
         <v>71</v>
       </c>
       <c r="E15" s="1">
-        <v>90</v>
+        <v>270</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
@@ -1129,7 +1129,7 @@
         <v>71</v>
       </c>
       <c r="E16" s="1">
-        <v>90</v>
+        <v>270</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
@@ -1146,7 +1146,7 @@
         <v>71</v>
       </c>
       <c r="E17" s="1">
-        <v>90</v>
+        <v>270</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
@@ -1163,7 +1163,7 @@
         <v>71</v>
       </c>
       <c r="E18" s="1">
-        <v>90</v>
+        <v>270</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
@@ -1180,7 +1180,7 @@
         <v>71</v>
       </c>
       <c r="E19" s="1">
-        <v>90</v>
+        <v>270</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
@@ -1197,7 +1197,7 @@
         <v>71</v>
       </c>
       <c r="E20" s="1">
-        <v>90</v>
+        <v>270</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
@@ -1214,7 +1214,7 @@
         <v>71</v>
       </c>
       <c r="E21" s="1">
-        <v>90</v>
+        <v>270</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
@@ -1231,7 +1231,7 @@
         <v>71</v>
       </c>
       <c r="E22" s="1">
-        <v>90</v>
+        <v>270</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
@@ -1248,7 +1248,7 @@
         <v>71</v>
       </c>
       <c r="E23" s="1">
-        <v>90</v>
+        <v>270</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
@@ -1265,7 +1265,7 @@
         <v>71</v>
       </c>
       <c r="E24" s="1">
-        <v>90</v>
+        <v>270</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
@@ -1282,7 +1282,7 @@
         <v>71</v>
       </c>
       <c r="E25" s="1">
-        <v>90</v>
+        <v>270</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
@@ -1299,7 +1299,7 @@
         <v>71</v>
       </c>
       <c r="E26" s="1">
-        <v>90</v>
+        <v>270</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
@@ -1316,7 +1316,7 @@
         <v>71</v>
       </c>
       <c r="E27" s="1">
-        <v>90</v>
+        <v>270</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
@@ -1333,7 +1333,7 @@
         <v>71</v>
       </c>
       <c r="E28" s="1">
-        <v>90</v>
+        <v>270</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
@@ -1350,7 +1350,7 @@
         <v>71</v>
       </c>
       <c r="E29" s="1">
-        <v>90</v>
+        <v>270</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
@@ -1367,7 +1367,7 @@
         <v>71</v>
       </c>
       <c r="E30" s="1">
-        <v>90</v>
+        <v>270</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
@@ -1384,7 +1384,7 @@
         <v>71</v>
       </c>
       <c r="E31" s="1">
-        <v>90</v>
+        <v>270</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
@@ -1401,7 +1401,7 @@
         <v>71</v>
       </c>
       <c r="E32" s="1">
-        <v>90</v>
+        <v>270</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
@@ -1418,7 +1418,7 @@
         <v>71</v>
       </c>
       <c r="E33" s="1">
-        <v>90</v>
+        <v>270</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
@@ -1434,8 +1434,8 @@
       <c r="D34" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E34">
-        <v>90</v>
+      <c r="E34" s="1">
+        <v>270</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
@@ -1451,8 +1451,8 @@
       <c r="D35" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E35">
-        <v>90</v>
+      <c r="E35" s="1">
+        <v>270</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
@@ -1468,8 +1468,8 @@
       <c r="D36" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E36">
-        <v>90</v>
+      <c r="E36" s="1">
+        <v>270</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
@@ -1485,8 +1485,8 @@
       <c r="D37" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E37">
-        <v>90</v>
+      <c r="E37" s="1">
+        <v>270</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
@@ -1502,8 +1502,8 @@
       <c r="D38" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E38">
-        <v>90</v>
+      <c r="E38" s="1">
+        <v>270</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
@@ -1519,8 +1519,8 @@
       <c r="D39" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E39">
-        <v>90</v>
+      <c r="E39" s="1">
+        <v>270</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
@@ -1536,8 +1536,8 @@
       <c r="D40" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E40">
-        <v>90</v>
+      <c r="E40" s="1">
+        <v>270</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
@@ -1553,8 +1553,8 @@
       <c r="D41" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E41">
-        <v>90</v>
+      <c r="E41" s="1">
+        <v>270</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.35">
@@ -1570,8 +1570,8 @@
       <c r="D42" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E42">
-        <v>90</v>
+      <c r="E42" s="1">
+        <v>270</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
@@ -1587,8 +1587,8 @@
       <c r="D43" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E43">
-        <v>90</v>
+      <c r="E43" s="1">
+        <v>270</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.35">
@@ -1604,8 +1604,8 @@
       <c r="D44" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E44">
-        <v>90</v>
+      <c r="E44" s="1">
+        <v>270</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
@@ -1621,8 +1621,8 @@
       <c r="D45" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E45">
-        <v>90</v>
+      <c r="E45" s="1">
+        <v>270</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
@@ -1638,8 +1638,8 @@
       <c r="D46" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E46">
-        <v>90</v>
+      <c r="E46" s="1">
+        <v>270</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
@@ -1655,8 +1655,8 @@
       <c r="D47" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E47">
-        <v>90</v>
+      <c r="E47" s="1">
+        <v>270</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.35">
@@ -1672,8 +1672,8 @@
       <c r="D48" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E48">
-        <v>90</v>
+      <c r="E48" s="1">
+        <v>270</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.35">
@@ -1689,8 +1689,8 @@
       <c r="D49" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E49">
-        <v>90</v>
+      <c r="E49" s="1">
+        <v>270</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.35">
@@ -1706,8 +1706,8 @@
       <c r="D50" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E50">
-        <v>90</v>
+      <c r="E50" s="1">
+        <v>270</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.35">
@@ -1723,8 +1723,8 @@
       <c r="D51" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E51">
-        <v>90</v>
+      <c r="E51" s="1">
+        <v>270</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.35">
@@ -1740,8 +1740,8 @@
       <c r="D52" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E52">
-        <v>90</v>
+      <c r="E52" s="1">
+        <v>270</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.35">
@@ -1757,8 +1757,8 @@
       <c r="D53" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E53">
-        <v>90</v>
+      <c r="E53" s="1">
+        <v>270</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.35">
@@ -1774,8 +1774,8 @@
       <c r="D54" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E54">
-        <v>90</v>
+      <c r="E54" s="1">
+        <v>270</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.35">
@@ -1791,8 +1791,8 @@
       <c r="D55" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E55">
-        <v>90</v>
+      <c r="E55" s="1">
+        <v>270</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.35">
@@ -1808,8 +1808,8 @@
       <c r="D56" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E56">
-        <v>90</v>
+      <c r="E56" s="1">
+        <v>270</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.35">
@@ -1825,8 +1825,8 @@
       <c r="D57" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E57">
-        <v>90</v>
+      <c r="E57" s="1">
+        <v>270</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.35">
@@ -1842,8 +1842,8 @@
       <c r="D58" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E58">
-        <v>90</v>
+      <c r="E58" s="1">
+        <v>270</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.35">
@@ -1859,8 +1859,8 @@
       <c r="D59" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E59">
-        <v>90</v>
+      <c r="E59" s="1">
+        <v>270</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.35">
@@ -1876,8 +1876,8 @@
       <c r="D60" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E60">
-        <v>90</v>
+      <c r="E60" s="1">
+        <v>270</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.35">
@@ -1893,8 +1893,8 @@
       <c r="D61" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E61">
-        <v>90</v>
+      <c r="E61" s="1">
+        <v>270</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.35">
@@ -1910,8 +1910,8 @@
       <c r="D62" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E62">
-        <v>90</v>
+      <c r="E62" s="1">
+        <v>270</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.35">
@@ -1927,8 +1927,8 @@
       <c r="D63" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E63">
-        <v>90</v>
+      <c r="E63" s="1">
+        <v>270</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.35">
@@ -1944,8 +1944,8 @@
       <c r="D64" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E64">
-        <v>90</v>
+      <c r="E64" s="1">
+        <v>270</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.35">
@@ -1961,8 +1961,8 @@
       <c r="D65" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E65">
-        <v>90</v>
+      <c r="E65" s="1">
+        <v>270</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.35">
@@ -1978,8 +1978,8 @@
       <c r="D66" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E66">
-        <v>90</v>
+      <c r="E66" s="1">
+        <v>270</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.35">
@@ -1995,8 +1995,8 @@
       <c r="D67" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E67">
-        <v>90</v>
+      <c r="E67" s="1">
+        <v>270</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.35">
@@ -2012,8 +2012,8 @@
       <c r="D68" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E68">
-        <v>90</v>
+      <c r="E68" s="1">
+        <v>270</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.35">
@@ -2029,8 +2029,8 @@
       <c r="D69" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E69">
-        <v>90</v>
+      <c r="E69" s="1">
+        <v>270</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.35">
@@ -2046,8 +2046,8 @@
       <c r="D70" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E70">
-        <v>90</v>
+      <c r="E70" s="1">
+        <v>270</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.35">
@@ -2063,8 +2063,8 @@
       <c r="D71" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E71">
-        <v>90</v>
+      <c r="E71" s="1">
+        <v>270</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.35">
@@ -2080,8 +2080,8 @@
       <c r="D72" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E72">
-        <v>90</v>
+      <c r="E72" s="1">
+        <v>270</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.35">
@@ -2097,8 +2097,8 @@
       <c r="D73" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E73">
-        <v>90</v>
+      <c r="E73" s="1">
+        <v>270</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.35">
@@ -2114,8 +2114,8 @@
       <c r="D74" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E74">
-        <v>90</v>
+      <c r="E74" s="1">
+        <v>270</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.35">
@@ -2131,8 +2131,8 @@
       <c r="D75" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E75">
-        <v>90</v>
+      <c r="E75" s="1">
+        <v>270</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.35">
@@ -2148,8 +2148,8 @@
       <c r="D76" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E76">
-        <v>90</v>
+      <c r="E76" s="1">
+        <v>270</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.35">
@@ -2165,8 +2165,8 @@
       <c r="D77" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E77">
-        <v>90</v>
+      <c r="E77" s="1">
+        <v>270</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.35">
@@ -2182,8 +2182,8 @@
       <c r="D78" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E78">
-        <v>90</v>
+      <c r="E78" s="1">
+        <v>270</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.35">
@@ -2199,8 +2199,8 @@
       <c r="D79" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E79">
-        <v>90</v>
+      <c r="E79" s="1">
+        <v>270</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.35">
@@ -2216,8 +2216,8 @@
       <c r="D80" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E80">
-        <v>90</v>
+      <c r="E80" s="1">
+        <v>270</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.35">
@@ -2233,8 +2233,8 @@
       <c r="D81" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E81">
-        <v>90</v>
+      <c r="E81" s="1">
+        <v>270</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.35">
@@ -2250,8 +2250,8 @@
       <c r="D82" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E82">
-        <v>90</v>
+      <c r="E82" s="1">
+        <v>270</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.35">
@@ -2267,8 +2267,8 @@
       <c r="D83" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E83">
-        <v>90</v>
+      <c r="E83" s="1">
+        <v>270</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.35">
@@ -2284,8 +2284,8 @@
       <c r="D84" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E84">
-        <v>90</v>
+      <c r="E84" s="1">
+        <v>270</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.35">
@@ -2301,8 +2301,8 @@
       <c r="D85" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E85">
-        <v>90</v>
+      <c r="E85" s="1">
+        <v>270</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.35">
@@ -2318,8 +2318,8 @@
       <c r="D86" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E86">
-        <v>90</v>
+      <c r="E86" s="1">
+        <v>270</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.35">
@@ -2335,8 +2335,8 @@
       <c r="D87" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E87">
-        <v>90</v>
+      <c r="E87" s="1">
+        <v>270</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.35">
@@ -2352,8 +2352,8 @@
       <c r="D88" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E88">
-        <v>90</v>
+      <c r="E88" s="1">
+        <v>270</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.35">
@@ -2369,8 +2369,8 @@
       <c r="D89" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E89">
-        <v>90</v>
+      <c r="E89" s="1">
+        <v>270</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.35">
@@ -2386,8 +2386,8 @@
       <c r="D90" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E90">
-        <v>90</v>
+      <c r="E90" s="1">
+        <v>270</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.35">
@@ -2403,8 +2403,8 @@
       <c r="D91" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E91">
-        <v>90</v>
+      <c r="E91" s="1">
+        <v>270</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.35">
@@ -2420,8 +2420,8 @@
       <c r="D92" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E92">
-        <v>90</v>
+      <c r="E92" s="1">
+        <v>270</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.35">
@@ -2437,8 +2437,8 @@
       <c r="D93" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E93">
-        <v>90</v>
+      <c r="E93" s="1">
+        <v>270</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.35">
@@ -2454,8 +2454,8 @@
       <c r="D94" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E94">
-        <v>90</v>
+      <c r="E94" s="1">
+        <v>270</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.35">
@@ -2471,8 +2471,8 @@
       <c r="D95" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E95">
-        <v>90</v>
+      <c r="E95" s="1">
+        <v>270</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.35">
@@ -2488,8 +2488,8 @@
       <c r="D96" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E96">
-        <v>90</v>
+      <c r="E96" s="1">
+        <v>270</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.35">
@@ -2505,8 +2505,8 @@
       <c r="D97" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E97">
-        <v>90</v>
+      <c r="E97" s="1">
+        <v>270</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.35">
@@ -2522,8 +2522,8 @@
       <c r="D98" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E98">
-        <v>90</v>
+      <c r="E98" s="1">
+        <v>270</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.35">
@@ -2539,8 +2539,8 @@
       <c r="D99" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E99">
-        <v>90</v>
+      <c r="E99" s="1">
+        <v>270</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.35">
@@ -2556,8 +2556,8 @@
       <c r="D100" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E100">
-        <v>90</v>
+      <c r="E100" s="1">
+        <v>270</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.35">
@@ -2573,8 +2573,8 @@
       <c r="D101" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E101">
-        <v>90</v>
+      <c r="E101" s="1">
+        <v>270</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.35">
@@ -2590,8 +2590,8 @@
       <c r="D102" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E102">
-        <v>90</v>
+      <c r="E102" s="1">
+        <v>270</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.35">
@@ -2607,8 +2607,8 @@
       <c r="D103" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E103">
-        <v>90</v>
+      <c r="E103" s="1">
+        <v>270</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.35">
@@ -2624,8 +2624,8 @@
       <c r="D104" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E104">
-        <v>90</v>
+      <c r="E104" s="1">
+        <v>270</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.35">
@@ -2641,8 +2641,8 @@
       <c r="D105" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E105">
-        <v>90</v>
+      <c r="E105" s="1">
+        <v>270</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.35">
@@ -2658,8 +2658,8 @@
       <c r="D106" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E106">
-        <v>90</v>
+      <c r="E106" s="1">
+        <v>270</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.35">
@@ -2675,8 +2675,8 @@
       <c r="D107" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E107">
-        <v>90</v>
+      <c r="E107" s="1">
+        <v>270</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.35">
@@ -2692,8 +2692,8 @@
       <c r="D108" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E108">
-        <v>90</v>
+      <c r="E108" s="1">
+        <v>270</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.35">
@@ -2709,8 +2709,8 @@
       <c r="D109" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E109">
-        <v>90</v>
+      <c r="E109" s="1">
+        <v>270</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.35">
@@ -2726,8 +2726,8 @@
       <c r="D110" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E110">
-        <v>90</v>
+      <c r="E110" s="1">
+        <v>270</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.35">
@@ -2743,8 +2743,8 @@
       <c r="D111" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E111">
-        <v>90</v>
+      <c r="E111" s="1">
+        <v>270</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.35">
@@ -2760,8 +2760,8 @@
       <c r="D112" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E112">
-        <v>90</v>
+      <c r="E112" s="1">
+        <v>270</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.35">
@@ -2777,8 +2777,8 @@
       <c r="D113" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E113">
-        <v>90</v>
+      <c r="E113" s="1">
+        <v>270</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.35">
@@ -2794,8 +2794,8 @@
       <c r="D114" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E114">
-        <v>90</v>
+      <c r="E114" s="1">
+        <v>270</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.35">
@@ -2811,8 +2811,8 @@
       <c r="D115" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E115">
-        <v>90</v>
+      <c r="E115" s="1">
+        <v>270</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.35">
@@ -2828,8 +2828,8 @@
       <c r="D116" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E116">
-        <v>90</v>
+      <c r="E116" s="1">
+        <v>270</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.35">
@@ -2845,8 +2845,8 @@
       <c r="D117" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E117">
-        <v>90</v>
+      <c r="E117" s="1">
+        <v>270</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.35">
@@ -2862,8 +2862,8 @@
       <c r="D118" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E118">
-        <v>90</v>
+      <c r="E118" s="1">
+        <v>270</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.35">
@@ -2879,8 +2879,8 @@
       <c r="D119" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E119">
-        <v>90</v>
+      <c r="E119" s="1">
+        <v>270</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.35">
@@ -2896,8 +2896,8 @@
       <c r="D120" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E120">
-        <v>90</v>
+      <c r="E120" s="1">
+        <v>270</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.35">
@@ -2913,8 +2913,8 @@
       <c r="D121" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E121">
-        <v>90</v>
+      <c r="E121" s="1">
+        <v>270</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.35">
@@ -2930,8 +2930,8 @@
       <c r="D122" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E122">
-        <v>90</v>
+      <c r="E122" s="1">
+        <v>270</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.35">
@@ -2947,8 +2947,8 @@
       <c r="D123" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E123">
-        <v>90</v>
+      <c r="E123" s="1">
+        <v>270</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.35">
@@ -2964,8 +2964,8 @@
       <c r="D124" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E124">
-        <v>90</v>
+      <c r="E124" s="1">
+        <v>270</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.35">
@@ -2981,8 +2981,8 @@
       <c r="D125" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E125">
-        <v>90</v>
+      <c r="E125" s="1">
+        <v>270</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.35">
@@ -2998,8 +2998,8 @@
       <c r="D126" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E126">
-        <v>90</v>
+      <c r="E126" s="1">
+        <v>270</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.35">
@@ -3015,8 +3015,8 @@
       <c r="D127" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E127">
-        <v>90</v>
+      <c r="E127" s="1">
+        <v>270</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.35">
@@ -3032,8 +3032,8 @@
       <c r="D128" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E128">
-        <v>90</v>
+      <c r="E128" s="1">
+        <v>270</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.35">
@@ -3049,8 +3049,8 @@
       <c r="D129" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E129">
-        <v>90</v>
+      <c r="E129" s="1">
+        <v>270</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.35">
@@ -3066,8 +3066,8 @@
       <c r="D130" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E130">
-        <v>90</v>
+      <c r="E130" s="1">
+        <v>270</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.35">
@@ -3083,8 +3083,8 @@
       <c r="D131" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="E131">
-        <v>90</v>
+      <c r="E131" s="1">
+        <v>270</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.35">

</xml_diff>